<commit_message>
update segmentation with new timing
</commit_message>
<xml_diff>
--- a/HR_Data/LWP2_0003_lab_timing.xlsx
+++ b/HR_Data/LWP2_0003_lab_timing.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CDRIVE\CTPC\LIVEWELL WEARTECH WEARABILITY ALL\WEARTECH compiled participant timings with participant info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CDRIVE\CTPC\LIVEWELL WEARTECH WEARABILITY ALL\WEARTECH compiled participant timings with participant info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -654,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +809,9 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4">
+        <v>0.52500000000000002</v>
+      </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
@@ -828,6 +830,9 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
+      <c r="B9" s="4">
+        <v>0.52638888888888891</v>
+      </c>
       <c r="C9" t="s">
         <v>28</v>
       </c>
@@ -894,6 +899,9 @@
       <c r="A12" t="s">
         <v>21</v>
       </c>
+      <c r="B12" s="4">
+        <v>0.53611111111111109</v>
+      </c>
       <c r="C12" t="s">
         <v>28</v>
       </c>
@@ -930,6 +938,9 @@
       <c r="A14" t="s">
         <v>1</v>
       </c>
+      <c r="B14" s="4">
+        <v>0.54375000000000007</v>
+      </c>
       <c r="C14" t="s">
         <v>25</v>
       </c>
@@ -951,6 +962,9 @@
       <c r="A15" t="s">
         <v>2</v>
       </c>
+      <c r="B15" s="4">
+        <v>0.5444444444444444</v>
+      </c>
       <c r="C15" t="s">
         <v>28</v>
       </c>
@@ -1008,6 +1022,9 @@
       <c r="A18" t="s">
         <v>5</v>
       </c>
+      <c r="B18" s="4">
+        <v>0.5541666666666667</v>
+      </c>
       <c r="C18" t="s">
         <v>30</v>
       </c>
@@ -1023,6 +1040,9 @@
       <c r="A19" t="s">
         <v>6</v>
       </c>
+      <c r="B19" s="4">
+        <v>0.5541666666666667</v>
+      </c>
       <c r="C19" t="s">
         <v>28</v>
       </c>
@@ -1091,6 +1111,9 @@
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.55972222222222223</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
update subj 03 and 05
</commit_message>
<xml_diff>
--- a/HR_Data/LWP2_0003_lab_timing.xlsx
+++ b/HR_Data/LWP2_0003_lab_timing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t>Event</t>
   </si>
@@ -213,9 +213,6 @@
     <t>NO TIMING DATA</t>
   </si>
   <si>
-    <t>NO EMA DATA</t>
-  </si>
-  <si>
     <t>Participant Info</t>
   </si>
   <si>
@@ -271,13 +268,19 @@
   </si>
   <si>
     <t>A00A7A</t>
+  </si>
+  <si>
+    <t>H5, A3, No C data, Stress 2, Yes</t>
+  </si>
+  <si>
+    <t>MISSED EMA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +290,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -327,7 +339,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -338,6 +349,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="21" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,7 +667,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,8 +694,8 @@
       <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>63</v>
+      <c r="I1" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -713,9 +725,9 @@
       <c r="F3" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="4"/>
       <c r="I3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -731,12 +743,12 @@
       <c r="F4" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="4"/>
       <c r="I4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" t="s">
         <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -752,17 +764,17 @@
       <c r="F5" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="6"/>
+      <c r="G5" s="5"/>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7">
-        <v>0.51527777777777783</v>
+      <c r="B6" s="6">
+        <v>0.51585648148148155</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -773,17 +785,17 @@
       <c r="F6" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="4"/>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4">
-        <v>0.51736111111111105</v>
+      <c r="B7" s="6">
+        <v>0.51715277777777779</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -794,23 +806,23 @@
       <c r="F7" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="4"/>
       <c r="I7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="L7" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4">
-        <v>0.52500000000000002</v>
+      <c r="B8" s="6">
+        <v>0.52479166666666666</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -821,23 +833,23 @@
       <c r="F8" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="J8" s="10" t="s">
-        <v>72</v>
+      <c r="G8" s="4"/>
+      <c r="J8" s="9" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4">
-        <v>0.52638888888888891</v>
+      <c r="B9" s="6">
+        <v>0.52606481481481482</v>
       </c>
       <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>62</v>
+      <c r="D9" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -845,17 +857,17 @@
       <c r="F9" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="J9" s="10" t="s">
-        <v>73</v>
+      <c r="G9" s="4"/>
+      <c r="J9" s="9" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="4">
-        <v>0.52777777777777779</v>
+      <c r="B10" s="6">
+        <v>0.52740740740740744</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
@@ -866,17 +878,17 @@
       <c r="F10" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="4"/>
       <c r="I10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="4">
-        <v>0.53541666666666665</v>
+      <c r="B11" s="6">
+        <v>0.53586805555555561</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
@@ -887,20 +899,20 @@
       <c r="F11" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="G11" s="4"/>
       <c r="I11" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" t="s">
         <v>75</v>
-      </c>
-      <c r="J11" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="4">
-        <v>0.53611111111111109</v>
+      <c r="B12" s="6">
+        <v>0.53657407407407409</v>
       </c>
       <c r="C12" t="s">
         <v>28</v>
@@ -911,14 +923,14 @@
       <c r="F12" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="4">
-        <v>0.53680555555555554</v>
+      <c r="B13" s="6">
+        <v>0.53744212962962956</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
@@ -929,17 +941,17 @@
       <c r="F13" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="6"/>
+      <c r="G13" s="5"/>
       <c r="I13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="4">
-        <v>0.54375000000000007</v>
+      <c r="B14" s="6">
+        <v>0.54388888888888887</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -950,20 +962,20 @@
       <c r="F14" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="5"/>
+      <c r="G14" s="4"/>
       <c r="I14" t="s">
+        <v>79</v>
+      </c>
+      <c r="J14" t="s">
         <v>80</v>
-      </c>
-      <c r="J14" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="4">
-        <v>0.5444444444444444</v>
+      <c r="B15" s="6">
+        <v>0.54488425925925921</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
@@ -974,20 +986,20 @@
       <c r="F15" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="4"/>
       <c r="I15" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" t="s">
         <v>78</v>
-      </c>
-      <c r="J15" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="4">
-        <v>0.54513888888888895</v>
+      <c r="B16" s="6">
+        <v>0.54540509259259262</v>
       </c>
       <c r="C16" t="s">
         <v>29</v>
@@ -998,14 +1010,14 @@
       <c r="F16" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="5"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="4">
-        <v>0.54722222222222217</v>
+      <c r="B17" s="6">
+        <v>0.54790509259259257</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
@@ -1016,14 +1028,14 @@
       <c r="F17" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="4">
-        <v>0.5541666666666667</v>
+      <c r="B18" s="6">
+        <v>0.554224537037037</v>
       </c>
       <c r="C18" t="s">
         <v>30</v>
@@ -1034,17 +1046,17 @@
       <c r="F18" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="4">
-        <v>0.5541666666666667</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
+      <c r="B19" s="10">
+        <v>0.554224537037037</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="E19">
         <v>17</v>
@@ -1052,14 +1064,14 @@
       <c r="F19" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="5"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="4">
-        <v>0.55486111111111114</v>
+      <c r="B20" s="6">
+        <v>0.55525462962962957</v>
       </c>
       <c r="C20" t="s">
         <v>31</v>
@@ -1070,14 +1082,14 @@
       <c r="F20" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="5"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="4">
-        <v>0.55763888888888891</v>
+      <c r="B21" s="6">
+        <v>0.55762731481481487</v>
       </c>
       <c r="C21" t="s">
         <v>32</v>
@@ -1088,14 +1100,14 @@
       <c r="F21" t="s">
         <v>56</v>
       </c>
-      <c r="G21" s="5"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="4">
-        <v>0.55902777777777779</v>
+      <c r="B22" s="6">
+        <v>0.55887731481481484</v>
       </c>
       <c r="C22" t="s">
         <v>27</v>
@@ -1106,14 +1118,14 @@
       <c r="F22" t="s">
         <v>48</v>
       </c>
-      <c r="G22" s="5"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="4">
-        <v>0.55972222222222223</v>
+      <c r="B23" s="6">
+        <v>0.55988425925925933</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
@@ -1124,14 +1136,14 @@
       <c r="F23" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="5"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="4">
-        <v>0.56180555555555556</v>
+      <c r="B24" s="6">
+        <v>0.56192129629629628</v>
       </c>
       <c r="C24" t="s">
         <v>33</v>
@@ -1142,14 +1154,14 @@
       <c r="F24" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="5"/>
+      <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="7">
-        <v>0.56319444444444444</v>
+      <c r="B25" s="6">
+        <v>0.56362268518518521</v>
       </c>
       <c r="E25">
         <v>23</v>
@@ -1157,7 +1169,7 @@
       <c r="F25" t="s">
         <v>58</v>
       </c>
-      <c r="G25" s="5"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E26">
@@ -1166,7 +1178,7 @@
       <c r="F26" t="s">
         <v>59</v>
       </c>
-      <c r="G26" s="5"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1178,7 +1190,7 @@
       <c r="F27" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="6"/>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E28">
@@ -1187,7 +1199,7 @@
       <c r="F28" t="s">
         <v>51</v>
       </c>
-      <c r="G28" s="5"/>
+      <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E29">
@@ -1196,7 +1208,7 @@
       <c r="F29" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="5"/>
+      <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E30">
@@ -1205,10 +1217,10 @@
       <c r="F30" t="s">
         <v>46</v>
       </c>
-      <c r="G30" s="6"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="8" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test on more subjects
</commit_message>
<xml_diff>
--- a/HR_Data/LWP2_0003_lab_timing.xlsx
+++ b/HR_Data/LWP2_0003_lab_timing.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CDRIVE\CTPC\LIVEWELL WEARTECH WEARABILITY ALL\WEARTECH compiled participant timings with participant info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophie\Documents\MATLAB\HeartRate\HR_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="In Lab" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
   <si>
     <t>Event</t>
   </si>
@@ -274,12 +274,15 @@
   </si>
   <si>
     <t>MISSED EMA</t>
+  </si>
+  <si>
+    <t>Task/Event number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -332,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -350,6 +353,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,563 +668,624 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
-    <col min="4" max="4" width="36.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" customWidth="1"/>
-    <col min="7" max="7" width="35" customWidth="1"/>
-    <col min="9" max="9" width="33.85546875" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+    <col min="2" max="3" width="28.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="33.85546875" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="I3" t="s">
+      <c r="J3" s="4"/>
+      <c r="K3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="I4" t="s">
+      <c r="J4" s="4"/>
+      <c r="K4" t="s">
         <v>64</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="3">
         <v>42626</v>
       </c>
-      <c r="E5">
+      <c r="C5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="I5" t="s">
+      <c r="J5" s="5"/>
+      <c r="K5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="6">
         <v>0.51585648148148155</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="I6" t="s">
+      <c r="J6" s="4"/>
+      <c r="K6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="6">
         <v>0.51715277777777779</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="11">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="I7" t="s">
+      <c r="J7" s="4"/>
+      <c r="K7" t="s">
         <v>68</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="M7" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="N7" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="6">
         <v>0.52479166666666666</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="11">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="4"/>
+      <c r="L8" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="6">
         <v>0.52606481481481482</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="11">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>7</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="4"/>
+      <c r="L9" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="6">
         <v>0.52740740740740744</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="11">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="I10" t="s">
+      <c r="J10" s="4"/>
+      <c r="K10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="6">
         <v>0.53586805555555561</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>27</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="I11" t="s">
+      <c r="J11" s="4"/>
+      <c r="K11" t="s">
         <v>74</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="6">
         <v>0.53657407407407409</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="11">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
         <v>28</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>10</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="6">
         <v>0.53744212962962956</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="11">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
         <v>24</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>11</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="I13" t="s">
+      <c r="J13" s="5"/>
+      <c r="K13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="6">
         <v>0.54388888888888887</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="11">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
         <v>25</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>12</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="I14" t="s">
+      <c r="J14" s="4"/>
+      <c r="K14" t="s">
         <v>79</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="6">
         <v>0.54488425925925921</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="11">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
         <v>28</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>13</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="I15" t="s">
+      <c r="J15" s="4"/>
+      <c r="K15" t="s">
         <v>77</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="6">
         <v>0.54540509259259262</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="11">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
         <v>29</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>14</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="6">
         <v>0.54790509259259257</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="11">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
         <v>24</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>15</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="6">
         <v>0.554224537037037</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="11">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
         <v>30</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>16</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="10">
         <v>0.554224537037037</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="11">
+        <v>13</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>17</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="6">
         <v>0.55525462962962957</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="11">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
         <v>31</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>18</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="6">
         <v>0.55762731481481487</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="11">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
         <v>32</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>19</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>56</v>
       </c>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="6">
         <v>0.55887731481481484</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="11">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s">
         <v>27</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>20</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>48</v>
       </c>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="6">
         <v>0.55988425925925933</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="11">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
         <v>28</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>21</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="6">
         <v>0.56192129629629628</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="11">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
         <v>33</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>22</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
       <c r="B25" s="6">
         <v>0.56362268518518521</v>
       </c>
-      <c r="E25">
+      <c r="C25" s="11"/>
+      <c r="F25">
         <v>23</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>58</v>
       </c>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E26">
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F26">
         <v>24</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>59</v>
       </c>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>25</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E28">
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F28">
         <v>26</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>51</v>
       </c>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E29">
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F29">
         <v>27</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E30">
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F30">
         <v>28</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>46</v>
       </c>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G31" s="8" t="s">
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J31" s="8" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>